<commit_message>
clean up and fix add fish form
</commit_message>
<xml_diff>
--- a/bio_diversity/static/report_templates/mortality_report_template.xlsx
+++ b/bio_diversity/static/report_templates/mortality_report_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Individuals" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="14">
   <si>
     <t>Collection</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Sample Number</t>
+  </si>
+  <si>
+    <t>Link</t>
   </si>
 </sst>
 </file>
@@ -918,7 +921,7 @@
   <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,11 +932,11 @@
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -992,6 +995,9 @@
       <c r="K2" s="6" t="s">
         <v>10</v>
       </c>
+      <c r="L2" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1001,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K2"/>
+  <dimension ref="A2:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,9 +1024,10 @@
     <col min="8" max="8" width="20.7109375" customWidth="1"/>
     <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="30.7109375" customWidth="1"/>
+    <col min="12" max="12" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
@@ -1053,6 +1060,9 @@
       </c>
       <c r="K2" s="6" t="s">
         <v>10</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1063,10 +1073,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J2"/>
+  <dimension ref="A2:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,9 +1088,11 @@
     <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" customWidth="1"/>
     <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" customWidth="1"/>
+    <col min="11" max="11" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -1110,6 +1122,9 @@
       </c>
       <c r="J2" s="6" t="s">
         <v>10</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>